<commit_message>
Major update of most of the package
</commit_message>
<xml_diff>
--- a/inst/extdata/importfileheader.xlsx
+++ b/inst/extdata/importfileheader.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thokal/Develop/SSRQc/inst/extdata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB206CD-6CB9-3745-9BE1-66D4A2C8DF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="28820" windowHeight="14900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,305 +25,317 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="95">
-  <si>
-    <t xml:space="preserve">DNA-analyseresultat</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
+  <si>
+    <t>DNA-analyseresultat</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">Individ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referanse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNAID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strekkode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RovbaseID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ArtsID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrøvestatusID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KjønnID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MetodeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VurderingID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KontrollstatusID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AnalysertAvID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merknad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IndividID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individnavn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReferanseID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referansetekst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1=Lodjur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1=Resultat erhållet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1=Hane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1=SVAN (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1=Dokumenterat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6=Laboratorium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1=Universitetet i Uppsala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tekst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1=NINA (Norsk institutt for naturforskn.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2=Järv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2=Inget resultat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2=Hona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2=LM002-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2=Universitetet i Lund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2=UIT (Universitetet i Tromsö)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3=Björn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3=Okänt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3=SVAN (Rev)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3=NINA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3=SVA (Statens veterinärmedicinska anstalt)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4=Varg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4=LECA (Bjørn)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4=Bioforsk Svanhovd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4=Forskningsindividnamn + chip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5=Kungsörn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5=LF001-02 (Järv)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5=Universitetet i Oslo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5=UiB (Universitetet i Bergen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6=Rödräv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6=LF001-03 (Järv)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6=LECA-Taberlet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6=UiO (Universitetet i Oslo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7=Fjällräv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7=LF002-02 (Varg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7=SVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7=Polisen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8=Hund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8=LF002-03 (Varg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8=SLU Grimsö</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8=NRM (Naturhistoriska riksmuseet)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9=Grävling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9=LF003-02 (Lodjur)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9=SLU Umeå</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9=VI (Veterinärinstitutet Norge)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10=Korp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10=LF003-03 (Lodjur)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10=Naturhistoriska riksmuseet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10=Gamla Rovbase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11=Kråka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11=NINA (Jerv)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11=Rovdjursforum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12=Hönsfågel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12=Grimsø (Varg 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12=Länsstyrelsens nummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13=Mårdhund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13=NINA (Varg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13=CITES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14=Okänd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14=NINA (Fjellrev)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14=Gamla SVA (Statens veterinärmedicinska anstalt)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15=Mink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15=SVAN (FOU)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15=Skandobs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16=SLU-SNP (Björn)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16=Naturvårdsverket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NB! Settes til 14 hvis
+    <t>Individ</t>
+  </si>
+  <si>
+    <t>Referanse</t>
+  </si>
+  <si>
+    <t>DNAID</t>
+  </si>
+  <si>
+    <t>Strekkode</t>
+  </si>
+  <si>
+    <t>RovbaseID</t>
+  </si>
+  <si>
+    <t>ArtsID</t>
+  </si>
+  <si>
+    <t>PrøvestatusID</t>
+  </si>
+  <si>
+    <t>KjønnID</t>
+  </si>
+  <si>
+    <t>MetodeID</t>
+  </si>
+  <si>
+    <t>VurderingID</t>
+  </si>
+  <si>
+    <t>KontrollstatusID</t>
+  </si>
+  <si>
+    <t>AnalysertAvID</t>
+  </si>
+  <si>
+    <t>Merknad</t>
+  </si>
+  <si>
+    <t>IndividID</t>
+  </si>
+  <si>
+    <t>Individnavn</t>
+  </si>
+  <si>
+    <t>ReferanseID</t>
+  </si>
+  <si>
+    <t>Referansetekst</t>
+  </si>
+  <si>
+    <t>1=Lodjur</t>
+  </si>
+  <si>
+    <t>1=Resultat erhållet</t>
+  </si>
+  <si>
+    <t>1=Hane</t>
+  </si>
+  <si>
+    <t>1=SVAN (1)</t>
+  </si>
+  <si>
+    <t>1=Dokumenterat</t>
+  </si>
+  <si>
+    <t>6=Laboratorium</t>
+  </si>
+  <si>
+    <t>1=Universitetet i Uppsala</t>
+  </si>
+  <si>
+    <t>Tekst</t>
+  </si>
+  <si>
+    <t>1=NINA (Norsk institutt for naturforskn.)</t>
+  </si>
+  <si>
+    <t>2=Järv</t>
+  </si>
+  <si>
+    <t>2=Inget resultat</t>
+  </si>
+  <si>
+    <t>2=Hona</t>
+  </si>
+  <si>
+    <t>2=LM002-02</t>
+  </si>
+  <si>
+    <t>2=Universitetet i Lund</t>
+  </si>
+  <si>
+    <t>2=UIT (Universitetet i Tromsö)</t>
+  </si>
+  <si>
+    <t>3=Björn</t>
+  </si>
+  <si>
+    <t>3=Okänt</t>
+  </si>
+  <si>
+    <t>3=SVAN (Rev)</t>
+  </si>
+  <si>
+    <t>3=NINA</t>
+  </si>
+  <si>
+    <t>3=SVA (Statens veterinärmedicinska anstalt)</t>
+  </si>
+  <si>
+    <t>4=Varg</t>
+  </si>
+  <si>
+    <t>4=LECA (Bjørn)</t>
+  </si>
+  <si>
+    <t>4=Bioforsk Svanhovd</t>
+  </si>
+  <si>
+    <t>4=Forskningsindividnamn + chip</t>
+  </si>
+  <si>
+    <t>5=Kungsörn</t>
+  </si>
+  <si>
+    <t>5=LF001-02 (Järv)</t>
+  </si>
+  <si>
+    <t>5=Universitetet i Oslo</t>
+  </si>
+  <si>
+    <t>5=UiB (Universitetet i Bergen)</t>
+  </si>
+  <si>
+    <t>6=Rödräv</t>
+  </si>
+  <si>
+    <t>6=LF001-03 (Järv)</t>
+  </si>
+  <si>
+    <t>6=LECA-Taberlet</t>
+  </si>
+  <si>
+    <t>6=UiO (Universitetet i Oslo)</t>
+  </si>
+  <si>
+    <t>7=Fjällräv</t>
+  </si>
+  <si>
+    <t>7=LF002-02 (Varg)</t>
+  </si>
+  <si>
+    <t>7=SVA</t>
+  </si>
+  <si>
+    <t>7=Polisen</t>
+  </si>
+  <si>
+    <t>8=Hund</t>
+  </si>
+  <si>
+    <t>8=LF002-03 (Varg)</t>
+  </si>
+  <si>
+    <t>8=SLU Grimsö</t>
+  </si>
+  <si>
+    <t>8=NRM (Naturhistoriska riksmuseet)</t>
+  </si>
+  <si>
+    <t>9=Grävling</t>
+  </si>
+  <si>
+    <t>9=LF003-02 (Lodjur)</t>
+  </si>
+  <si>
+    <t>9=SLU Umeå</t>
+  </si>
+  <si>
+    <t>9=VI (Veterinärinstitutet Norge)</t>
+  </si>
+  <si>
+    <t>10=Korp</t>
+  </si>
+  <si>
+    <t>10=LF003-03 (Lodjur)</t>
+  </si>
+  <si>
+    <t>10=Naturhistoriska riksmuseet</t>
+  </si>
+  <si>
+    <t>10=Gamla Rovbase</t>
+  </si>
+  <si>
+    <t>11=Kråka</t>
+  </si>
+  <si>
+    <t>11=NINA (Jerv)</t>
+  </si>
+  <si>
+    <t>11=Rovdjursforum</t>
+  </si>
+  <si>
+    <t>12=Hönsfågel</t>
+  </si>
+  <si>
+    <t>12=Grimsø (Varg 1)</t>
+  </si>
+  <si>
+    <t>12=Länsstyrelsens nummer</t>
+  </si>
+  <si>
+    <t>13=Mårdhund</t>
+  </si>
+  <si>
+    <t>13=NINA (Varg)</t>
+  </si>
+  <si>
+    <t>13=CITES</t>
+  </si>
+  <si>
+    <t>14=Okänd</t>
+  </si>
+  <si>
+    <t>14=NINA (Fjellrev)</t>
+  </si>
+  <si>
+    <t>14=Gamla SVA (Statens veterinärmedicinska anstalt)</t>
+  </si>
+  <si>
+    <t>15=Mink</t>
+  </si>
+  <si>
+    <t>15=SVAN (FOU)</t>
+  </si>
+  <si>
+    <t>15=Skandobs</t>
+  </si>
+  <si>
+    <t>16=SLU-SNP (Björn)</t>
+  </si>
+  <si>
+    <t>16=Naturvårdsverket</t>
+  </si>
+  <si>
+    <t>NB! Settes til 14 hvis
 PrøvestatusID=2</t>
   </si>
   <si>
-    <t xml:space="preserve">NB! Settes til 3 hvis
+    <t>NB! Settes til 3 hvis
 PrøvestatusID=2</t>
   </si>
   <si>
-    <t xml:space="preserve">17=NINA (Kongeørn)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NB! Fylles ikke 
+    <t>17=NINA (Kongeørn)</t>
+  </si>
+  <si>
+    <t>NB! Fylles ikke 
 ut hvis 
 PrøvestatusID=2</t>
   </si>
   <si>
-    <t xml:space="preserve">17=Länsstyrelsens diarienummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18=NH-2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18=Laboratoriereferens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19=NH-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19=Prov-ID från Laboratorie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20=Grimsö (Varg SNP V1.1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20=FeltApp</t>
+    <t>17=Länsstyrelsens diarienummer</t>
+  </si>
+  <si>
+    <t>18=NH-2015</t>
+  </si>
+  <si>
+    <t>18=Laboratoriereferens</t>
+  </si>
+  <si>
+    <t>19=NH-1</t>
+  </si>
+  <si>
+    <t>19=Prov-ID från Laboratorie</t>
+  </si>
+  <si>
+    <t>20=Grimsö (Varg SNP V1.1)</t>
+  </si>
+  <si>
+    <t>20=FeltApp</t>
+  </si>
+  <si>
+    <t>RB-individ</t>
+  </si>
+  <si>
+    <t>Län</t>
+  </si>
+  <si>
+    <t>NRM-individ</t>
+  </si>
+  <si>
+    <t>Rb-kön</t>
+  </si>
+  <si>
+    <t>To Remove before sharing to rovbase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -327,26 +344,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -361,7 +363,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,9 +382,15 @@
         <bgColor rgb="FFB4C7E7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -390,61 +398,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -503,28 +474,356 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:O23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.11"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,8 +869,11 @@
       <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -617,8 +919,20 @@
       <c r="O2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -656,8 +970,12 @@
         <v>27</v>
       </c>
       <c r="O3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -685,8 +1003,12 @@
         <v>33</v>
       </c>
       <c r="O4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -712,8 +1034,12 @@
         <v>38</v>
       </c>
       <c r="O5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -737,8 +1063,12 @@
         <v>42</v>
       </c>
       <c r="O6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -762,8 +1092,12 @@
         <v>46</v>
       </c>
       <c r="O7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -787,8 +1121,12 @@
         <v>50</v>
       </c>
       <c r="O8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -812,8 +1150,12 @@
         <v>54</v>
       </c>
       <c r="O9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -837,8 +1179,12 @@
         <v>58</v>
       </c>
       <c r="O10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -862,8 +1208,12 @@
         <v>62</v>
       </c>
       <c r="O11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -887,8 +1237,12 @@
         <v>66</v>
       </c>
       <c r="O12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -910,8 +1264,12 @@
         <v>69</v>
       </c>
       <c r="O13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -933,8 +1291,12 @@
         <v>72</v>
       </c>
       <c r="O14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -956,8 +1318,12 @@
         <v>75</v>
       </c>
       <c r="O15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -979,8 +1345,12 @@
         <v>78</v>
       </c>
       <c r="O16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1002,8 +1372,12 @@
         <v>81</v>
       </c>
       <c r="O17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1023,8 +1397,12 @@
         <v>83</v>
       </c>
       <c r="O18" s="3"/>
-    </row>
-    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+    </row>
+    <row r="19" spans="1:19" ht="80" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1052,8 +1430,12 @@
         <v>88</v>
       </c>
       <c r="O19" s="3"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1073,8 +1455,12 @@
         <v>90</v>
       </c>
       <c r="O20" s="3"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1094,8 +1480,12 @@
         <v>92</v>
       </c>
       <c r="O21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1115,8 +1505,12 @@
         <v>94</v>
       </c>
       <c r="O22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
@@ -1162,12 +1556,23 @@
       <c r="O23" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="P23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>